<commit_message>
update check and vhead/chead
</commit_message>
<xml_diff>
--- a/excel/excel_demo/regbank_demo.xlsx
+++ b/excel/excel_demo/regbank_demo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
   <si>
     <t>Access_Type</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>lock_field_0</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>lock field 0</t>
@@ -378,12 +375,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -393,6 +384,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -551,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -562,19 +559,19 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -583,55 +580,40 @@
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -953,9 +935,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="29" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="30" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="29" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="24" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="25" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="24" width="10.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="10.147857142857141" customWidth="1" bestFit="1"/>
@@ -963,9 +945,9 @@
     <col min="8" max="8" style="3" width="16.005" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="3" width="13.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="36.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="29" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="29" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="29" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="24" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="24" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="24" width="13.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1000,897 +982,889 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>8</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>16</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="b">
-        <v>0</v>
+      <c r="B6" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17" t="s">
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="17"/>
+      <c r="M11" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="21"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="21"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="17" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L16" s="20" t="s">
+      <c r="L16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="M16" s="20"/>
+      <c r="M16" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="21"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="21"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="21"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="21"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20" t="s">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="M21" s="20"/>
+      <c r="M21" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="21"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="21"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="17" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="21"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="21"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17" t="s">
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17" t="s">
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17" t="s">
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17" t="s">
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="17"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="26" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="16"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="17"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="26" t="s">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="16"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="25" t="s">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="16"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="17"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="17"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="17"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="17"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="17"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="17"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="17"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="17"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="27"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1898,9 +1872,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
update vhead & chead
</commit_message>
<xml_diff>
--- a/excel/excel_demo/regbank_demo.xlsx
+++ b/excel/excel_demo/regbank_demo.xlsx
@@ -365,7 +365,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,12 +384,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -548,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -603,9 +597,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -935,9 +926,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="24" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="25" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="24" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="23" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="24" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="23" width="10.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="10.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="10.147857142857141" customWidth="1" bestFit="1"/>
@@ -945,9 +936,9 @@
     <col min="8" max="8" style="3" width="16.005" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="3" width="13.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="36.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="24" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="24" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="24" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="23" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="23" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="23" width="13.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1048,7 +1039,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="16"/>
@@ -1077,45 +1068,45 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1156,7 +1147,7 @@
       <c r="A11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1178,9 +1169,9 @@
       <c r="M11" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="19"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
         <v>66</v>
       </c>
@@ -1207,9 +1198,9 @@
       <c r="M12" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="19"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="19"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
         <v>70</v>
       </c>
@@ -1236,9 +1227,9 @@
       <c r="M13" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="19"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="19"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="16" t="s">
         <v>74</v>
       </c>
@@ -1265,9 +1256,9 @@
       <c r="M14" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="19"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="19"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
         <v>77</v>
       </c>
@@ -1297,7 +1288,7 @@
       <c r="A16" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>82</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -1321,9 +1312,9 @@
       <c r="M16" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="19"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="19"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="16" t="s">
         <v>66</v>
       </c>
@@ -1352,9 +1343,9 @@
       <c r="M17" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="19"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="19"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="16" t="s">
         <v>70</v>
       </c>
@@ -1383,9 +1374,9 @@
       <c r="M18" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="19"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="19"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="16" t="s">
         <v>74</v>
       </c>
@@ -1412,9 +1403,9 @@
       <c r="M19" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="19"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="19"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
         <v>77</v>
       </c>
@@ -1436,7 +1427,7 @@
       <c r="J20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="K20" s="19"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
@@ -1444,7 +1435,7 @@
       <c r="A21" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -1466,9 +1457,9 @@
       <c r="M21" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="19"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="19"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
         <v>66</v>
       </c>
@@ -1495,9 +1486,9 @@
       <c r="M22" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="19"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="19"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="16" t="s">
         <v>70</v>
       </c>
@@ -1524,9 +1515,9 @@
       <c r="M23" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="19"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
         <v>74</v>
       </c>
@@ -1553,9 +1544,9 @@
       <c r="M24" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="19"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="19"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
         <v>77</v>
       </c>
@@ -1587,7 +1578,7 @@
       <c r="A26" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>96</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -1616,7 +1607,7 @@
       <c r="A27" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="16" t="s">
@@ -1645,7 +1636,7 @@
       <c r="A28" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -1666,7 +1657,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="16"/>
-      <c r="B29" s="23"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16" t="s">
         <v>106</v>
@@ -1687,7 +1678,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="16"/>
-      <c r="B30" s="23"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16" t="s">
         <v>108</v>
@@ -1710,7 +1701,7 @@
       <c r="A31" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>112</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -1731,7 +1722,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="16"/>
-      <c r="B32" s="23"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
         <v>106</v>
@@ -1752,7 +1743,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="16"/>
-      <c r="B33" s="23"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16" t="s">
         <v>108</v>
@@ -1773,7 +1764,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="16"/>
-      <c r="B34" s="23"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1788,7 +1779,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="16"/>
-      <c r="B35" s="23"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1803,7 +1794,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="16"/>
-      <c r="B36" s="23"/>
+      <c r="B36" s="22"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1818,7 +1809,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="16"/>
-      <c r="B37" s="23"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1833,7 +1824,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="16"/>
-      <c r="B38" s="23"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1848,7 +1839,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="16"/>
-      <c r="B39" s="23"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1863,7 +1854,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="16"/>
-      <c r="B40" s="23"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="16"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>

</xml_diff>